<commit_message>
Refactor service number extraction and enhance plantilla generation with additional fields
</commit_message>
<xml_diff>
--- a/checar.xlsx
+++ b/checar.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,10 +425,11 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AJ5"/>
+  <dimension ref="A1:Z5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -436,866 +437,572 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Nombre</t>
+          <t>No. Doc</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Version</t>
+          <t>Posicion</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Serie</t>
+          <t>Tipo de documento</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Folio</t>
+          <t>Tipo de asignación</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Fecha</t>
+          <t>Asignación</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Metodo_de_pago</t>
+          <t>Proveedor</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>Forma_de_pago</t>
+          <t>Empresa compradora</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
+          <t>No. Servicio</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
           <t>Moneda</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>Tipo_de_comprobante</t>
-        </is>
-      </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>Exportacion</t>
+          <t>Documento externo</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>TipoRelacion</t>
+          <t>Folio fiscal</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>UUID_relacionado</t>
+          <t>Fecha de recepción</t>
         </is>
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>Rfc_emisor</t>
+          <t>Fecha de factura</t>
         </is>
       </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
-          <t>Nombre_emisor</t>
+          <t>Fecha de contabilización</t>
         </is>
       </c>
       <c r="O1" s="1" t="inlineStr">
         <is>
-          <t>Regimen_fiscal_emisor</t>
+          <t>Fecha de vencimiento</t>
         </is>
       </c>
       <c r="P1" s="1" t="inlineStr">
         <is>
-          <t>Domicilio_fiscal_receptor</t>
+          <t>ID de producto</t>
         </is>
       </c>
       <c r="Q1" s="1" t="inlineStr">
         <is>
-          <t>Rfc_receptor</t>
+          <t>Cantidad</t>
         </is>
       </c>
       <c r="R1" s="1" t="inlineStr">
         <is>
-          <t>Nombre_receptor</t>
+          <t>Precio neto</t>
         </is>
       </c>
       <c r="S1" s="1" t="inlineStr">
         <is>
-          <t>Regimen_fiscal_receptor</t>
+          <t>Código de impuesto</t>
         </is>
       </c>
       <c r="T1" s="1" t="inlineStr">
         <is>
-          <t>Uso_de_CFDI</t>
+          <t>Código de retención</t>
         </is>
       </c>
       <c r="U1" s="1" t="inlineStr">
         <is>
-          <t>Clave_ProdServ</t>
+          <t>Importe de impuesto</t>
         </is>
       </c>
       <c r="V1" s="1" t="inlineStr">
         <is>
-          <t>Descripcion</t>
+          <t>Nombre archivo XML</t>
         </is>
       </c>
       <c r="W1" s="1" t="inlineStr">
         <is>
-          <t>Importe</t>
+          <t>Descripción</t>
         </is>
       </c>
       <c r="X1" s="1" t="inlineStr">
         <is>
-          <t>Objeto_de_impuesto</t>
+          <t>Observación asignación de producto</t>
         </is>
       </c>
       <c r="Y1" s="1" t="inlineStr">
         <is>
-          <t>Base_IVA</t>
+          <t>Clave de producto o servicio</t>
         </is>
       </c>
       <c r="Z1" s="1" t="inlineStr">
         <is>
-          <t>Impuesto_IVA</t>
-        </is>
-      </c>
-      <c r="AA1" s="1" t="inlineStr">
-        <is>
-          <t>Tasa_o_cuota_IVA</t>
-        </is>
-      </c>
-      <c r="AB1" s="1" t="inlineStr">
-        <is>
-          <t>Importe_IVA</t>
-        </is>
-      </c>
-      <c r="AC1" s="1" t="inlineStr">
-        <is>
-          <t>Base_retencion</t>
-        </is>
-      </c>
-      <c r="AD1" s="1" t="inlineStr">
-        <is>
-          <t>Impuesto_retencion</t>
-        </is>
-      </c>
-      <c r="AE1" s="1" t="inlineStr">
-        <is>
-          <t>Tasa_o_cuota_retencion</t>
-        </is>
-      </c>
-      <c r="AF1" s="1" t="inlineStr">
-        <is>
-          <t>Importe_retencion</t>
-        </is>
-      </c>
-      <c r="AG1" s="1" t="inlineStr">
-        <is>
-          <t>Carta_porte</t>
-        </is>
-      </c>
-      <c r="AH1" s="1" t="inlineStr">
-        <is>
-          <t>Carta_porte_version</t>
-        </is>
-      </c>
-      <c r="AI1" s="1" t="inlineStr">
-        <is>
-          <t>UUID</t>
-        </is>
-      </c>
-      <c r="AJ1" s="1" t="inlineStr">
-        <is>
-          <t>Observaciones</t>
+          <t>Descripción concepto XML</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>24-002529-47950.xml</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>4.0</t>
-        </is>
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="n">
+        <v>1</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>CPN</t>
+          <t>Factura</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>47950</t>
+          <t>CC</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2024-02-01T21:46:33</t>
+          <t>MLG1405</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>PPD</t>
+          <t>T00943</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>99</t>
+          <t>MLG1000</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>USD</t>
+          <t>24-030477</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>I</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>01</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr"/>
+          <t>MXN</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr"/>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>EFDFED4B-8E21-1B43-B155-15BB076CDE38</t>
+        </is>
+      </c>
       <c r="L2" t="inlineStr"/>
       <c r="M2" t="inlineStr">
         <is>
-          <t>ESA970515374</t>
+          <t>05/11/2024</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>ESPECIALIZADOS SAGOT</t>
-        </is>
-      </c>
-      <c r="O2" t="inlineStr">
-        <is>
-          <t>624</t>
-        </is>
-      </c>
+          <t>05/11/2024</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr"/>
       <c r="P2" t="inlineStr">
         <is>
-          <t>03900</t>
-        </is>
-      </c>
-      <c r="Q2" t="inlineStr">
-        <is>
-          <t>MIN1002195D0</t>
-        </is>
+          <t>INDETERMINADO</t>
+        </is>
+      </c>
+      <c r="Q2" t="n">
+        <v>1</v>
       </c>
       <c r="R2" t="inlineStr">
         <is>
-          <t>MULTILOG INTERNACIONAL</t>
+          <t>1693.01</t>
         </is>
       </c>
       <c r="S2" t="inlineStr">
         <is>
-          <t>601</t>
+          <t>3</t>
         </is>
       </c>
       <c r="T2" t="inlineStr">
         <is>
-          <t>G03</t>
+          <t>G1I</t>
         </is>
       </c>
       <c r="U2" t="inlineStr">
         <is>
-          <t>78101806</t>
+          <t>270.88</t>
         </is>
       </c>
       <c r="V2" t="inlineStr">
         <is>
-          <t>VACIO</t>
-        </is>
-      </c>
-      <c r="W2" t="inlineStr">
-        <is>
-          <t>160.00</t>
-        </is>
-      </c>
+          <t>24-030477-779471674450001</t>
+        </is>
+      </c>
+      <c r="W2" t="inlineStr"/>
       <c r="X2" t="inlineStr">
         <is>
-          <t>02</t>
+          <t>(!) No se encontró coincidencia en la tabla de asignación</t>
         </is>
       </c>
       <c r="Y2" t="inlineStr">
         <is>
-          <t>160.00</t>
+          <t>81141601</t>
         </is>
       </c>
       <c r="Z2" t="inlineStr">
         <is>
-          <t>002</t>
-        </is>
-      </c>
-      <c r="AA2" t="inlineStr">
-        <is>
-          <t>0.000000</t>
-        </is>
-      </c>
-      <c r="AB2" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="AC2" t="inlineStr">
-        <is>
-          <t>160.00|</t>
-        </is>
-      </c>
-      <c r="AD2" t="inlineStr">
-        <is>
-          <t>002|</t>
-        </is>
-      </c>
-      <c r="AE2" t="inlineStr">
-        <is>
-          <t>0.000000|</t>
-        </is>
-      </c>
-      <c r="AF2" t="inlineStr">
-        <is>
-          <t>0.00|</t>
-        </is>
-      </c>
-      <c r="AG2" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="AH2" t="inlineStr">
-        <is>
-          <t>Sin carta porte</t>
-        </is>
-      </c>
-      <c r="AI2" t="inlineStr">
-        <is>
-          <t>5145FD6C-69EB-4624-B16C-BF1176B474E1</t>
-        </is>
-      </c>
-      <c r="AJ2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Retención incorrecta para clave de prod. y serv.| Carta Porte no anexa para clave de prod. y serv.| </t>
+          <t>SERVICIOS DE LOGISTICA (MX)/LOGISTIC SERVICES (MX)</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>24-011101-2800.xml</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>4.0</t>
-        </is>
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="n">
+        <v>1</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>VIZ</t>
+          <t>Factura</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>2800</t>
+          <t>CC</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>2024-05-06T12:06:00</t>
+          <t>MLG1405</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>PPD</t>
+          <t>T00943</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>99</t>
+          <t>MLG1000</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>USD</t>
+          <t>24-030480</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>I</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>01</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr"/>
+          <t>MXN</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr"/>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>E80D77EB-575A-B645-A714-21A9A53E5255</t>
+        </is>
+      </c>
       <c r="L3" t="inlineStr"/>
       <c r="M3" t="inlineStr">
         <is>
-          <t>TTV960430UY4</t>
+          <t>05/11/2024</t>
         </is>
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>TRANSPORTES TERRESTRES VALDEZ</t>
-        </is>
-      </c>
-      <c r="O3" t="inlineStr">
-        <is>
-          <t>624</t>
-        </is>
-      </c>
+          <t>05/11/2024</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr"/>
       <c r="P3" t="inlineStr">
         <is>
-          <t>03900</t>
-        </is>
-      </c>
-      <c r="Q3" t="inlineStr">
-        <is>
-          <t>MIN1002195D0</t>
-        </is>
+          <t>INDETERMINADO</t>
+        </is>
+      </c>
+      <c r="Q3" t="n">
+        <v>1</v>
       </c>
       <c r="R3" t="inlineStr">
         <is>
-          <t>MULTILOG INTERNACIONAL</t>
+          <t>1148.99</t>
         </is>
       </c>
       <c r="S3" t="inlineStr">
         <is>
-          <t>601</t>
+          <t>3</t>
         </is>
       </c>
       <c r="T3" t="inlineStr">
         <is>
-          <t>G03</t>
+          <t>G1I</t>
         </is>
       </c>
       <c r="U3" t="inlineStr">
         <is>
-          <t>78141902</t>
+          <t>183.84</t>
         </is>
       </c>
       <c r="V3" t="inlineStr">
         <is>
-          <t>RENTA DE CONTENEDORES CERRADOS Y DEMORAS DEMORA 24-011101</t>
-        </is>
-      </c>
-      <c r="W3" t="inlineStr">
-        <is>
-          <t>250.000000</t>
-        </is>
-      </c>
+          <t>24-030480-779474725969001</t>
+        </is>
+      </c>
+      <c r="W3" t="inlineStr"/>
       <c r="X3" t="inlineStr">
         <is>
-          <t>02</t>
+          <t>(!) No se encontró coincidencia en la tabla de asignación</t>
         </is>
       </c>
       <c r="Y3" t="inlineStr">
         <is>
-          <t>250.00</t>
+          <t>81141601</t>
         </is>
       </c>
       <c r="Z3" t="inlineStr">
         <is>
-          <t>002</t>
-        </is>
-      </c>
-      <c r="AA3" t="inlineStr">
-        <is>
-          <t>0.160000</t>
-        </is>
-      </c>
-      <c r="AB3" t="inlineStr">
-        <is>
-          <t>40.00</t>
-        </is>
-      </c>
-      <c r="AC3" t="inlineStr"/>
-      <c r="AD3" t="inlineStr"/>
-      <c r="AE3" t="inlineStr"/>
-      <c r="AF3" t="inlineStr"/>
-      <c r="AG3" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="AH3" t="inlineStr">
-        <is>
-          <t>Sin carta porte</t>
-        </is>
-      </c>
-      <c r="AI3" t="inlineStr">
-        <is>
-          <t>DFCD1455-F781-4A4C-B489-48ECBF86D300</t>
-        </is>
-      </c>
-      <c r="AJ3" t="inlineStr"/>
+          <t>SERVICIOS DE LOGISTICA (MX)/LOGISTIC SERVICES (MX)</t>
+        </is>
+      </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>24017624 - 30765.xml</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>4.0</t>
-        </is>
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="n">
+        <v>1</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>VER</t>
+          <t>Factura</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>30765</t>
+          <t>CC</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>2024-06-28T17:58:34</t>
+          <t>MLG1405</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>PPD</t>
+          <t>T00943</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>99</t>
+          <t>MLG1000</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
+          <t>24-031142</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
           <t>MXN</t>
         </is>
       </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>I</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>01</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr"/>
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>BD665673-1EAF-4D46-A3F2-EECA0C64AC6D</t>
+        </is>
+      </c>
       <c r="L4" t="inlineStr"/>
       <c r="M4" t="inlineStr">
         <is>
-          <t>FMF901004UZ9</t>
+          <t>05/11/2024</t>
         </is>
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>FLETES Y MATERIALES FORSIS</t>
-        </is>
-      </c>
-      <c r="O4" t="inlineStr">
-        <is>
-          <t>624</t>
-        </is>
-      </c>
+          <t>05/11/2024</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr"/>
       <c r="P4" t="inlineStr">
         <is>
-          <t>03900</t>
-        </is>
-      </c>
-      <c r="Q4" t="inlineStr">
-        <is>
-          <t>MIN1002195D0</t>
-        </is>
+          <t>INDETERMINADO</t>
+        </is>
+      </c>
+      <c r="Q4" t="n">
+        <v>1</v>
       </c>
       <c r="R4" t="inlineStr">
         <is>
-          <t>MULTILOG INTERNACIONAL</t>
+          <t>21272.92</t>
         </is>
       </c>
       <c r="S4" t="inlineStr">
         <is>
-          <t>601</t>
+          <t>3</t>
         </is>
       </c>
       <c r="T4" t="inlineStr">
         <is>
-          <t>G03</t>
+          <t>G1I</t>
         </is>
       </c>
       <c r="U4" t="inlineStr">
         <is>
-          <t>78101800</t>
+          <t>3403.67</t>
         </is>
       </c>
       <c r="V4" t="inlineStr">
         <is>
-          <t>DE 1 X 20 DC (HLBU2552560) DE VERACRUZ, VER. A CUAUTITLAN, EDO. DE MEXICO.</t>
-        </is>
-      </c>
-      <c r="W4" t="inlineStr">
-        <is>
-          <t>29650.0</t>
-        </is>
-      </c>
+          <t>24-031142-779567411325001</t>
+        </is>
+      </c>
+      <c r="W4" t="inlineStr"/>
       <c r="X4" t="inlineStr">
         <is>
-          <t>02</t>
+          <t>(!) No se encontró coincidencia en la tabla de asignación</t>
         </is>
       </c>
       <c r="Y4" t="inlineStr">
         <is>
-          <t>29650.0</t>
+          <t>81141601</t>
         </is>
       </c>
       <c r="Z4" t="inlineStr">
         <is>
-          <t>002</t>
-        </is>
-      </c>
-      <c r="AA4" t="inlineStr">
-        <is>
-          <t>0.160000</t>
-        </is>
-      </c>
-      <c r="AB4" t="inlineStr">
-        <is>
-          <t>4744.0</t>
-        </is>
-      </c>
-      <c r="AC4" t="inlineStr">
-        <is>
-          <t>29650.0|</t>
-        </is>
-      </c>
-      <c r="AD4" t="inlineStr">
-        <is>
-          <t>002|</t>
-        </is>
-      </c>
-      <c r="AE4" t="inlineStr">
-        <is>
-          <t>0.040000|</t>
-        </is>
-      </c>
-      <c r="AF4" t="inlineStr">
-        <is>
-          <t>1186.0|</t>
-        </is>
-      </c>
-      <c r="AG4" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="AH4" t="inlineStr">
-        <is>
-          <t>Sin carta porte</t>
-        </is>
-      </c>
-      <c r="AI4" t="inlineStr">
-        <is>
-          <t>361e4e73-5a3b-4617-9544-6e85b3586ab8</t>
-        </is>
-      </c>
-      <c r="AJ4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Carta Porte no anexa para clave de prod. y serv.| </t>
+          <t>SERVICIOS DE LOGISTICA (MX)/LOGISTIC SERVICES (MX)</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>24_004629_5850.xml</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>4.0</t>
-        </is>
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="n">
+        <v>1</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>CPM</t>
+          <t>Factura</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>5850</t>
+          <t>CC</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>2024-03-27T15:35:38</t>
+          <t>MLG1405</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>PPD</t>
+          <t>T00943</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>99</t>
+          <t>MLG1000</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
+          <t>24-031264</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
           <t>MXN</t>
         </is>
       </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>I</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>01</t>
-        </is>
-      </c>
+      <c r="J5" t="inlineStr"/>
       <c r="K5" t="inlineStr">
         <is>
-          <t>04</t>
-        </is>
-      </c>
-      <c r="L5" t="inlineStr">
-        <is>
-          <t>33b6e826-d29d-4eea-b27a-000e1ac6b0bf</t>
-        </is>
-      </c>
+          <t>AA872B02-4680-B54D-A486-0E8C3905A4B3</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr"/>
       <c r="M5" t="inlineStr">
         <is>
-          <t>ACT110316S47</t>
+          <t>05/11/2024</t>
         </is>
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>AUTOTRANSPORTES DE CARGA THR</t>
-        </is>
-      </c>
-      <c r="O5" t="inlineStr">
-        <is>
-          <t>624</t>
-        </is>
-      </c>
+          <t>05/11/2024</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr"/>
       <c r="P5" t="inlineStr">
         <is>
-          <t>03900</t>
-        </is>
-      </c>
-      <c r="Q5" t="inlineStr">
-        <is>
-          <t>MIN1002195D0</t>
-        </is>
+          <t>INDETERMINADO</t>
+        </is>
+      </c>
+      <c r="Q5" t="n">
+        <v>1</v>
       </c>
       <c r="R5" t="inlineStr">
         <is>
-          <t>MULTILOG INTERNACIONAL</t>
+          <t>1593.50</t>
         </is>
       </c>
       <c r="S5" t="inlineStr">
         <is>
-          <t>601</t>
+          <t>3</t>
         </is>
       </c>
       <c r="T5" t="inlineStr">
         <is>
-          <t>G03</t>
+          <t>G1I</t>
         </is>
       </c>
       <c r="U5" t="inlineStr">
         <is>
-          <t>78101802</t>
+          <t>254.96</t>
         </is>
       </c>
       <c r="V5" t="inlineStr">
         <is>
-          <t>SERVICIO DE FLETE</t>
-        </is>
-      </c>
-      <c r="W5" t="inlineStr">
-        <is>
-          <t>16150.00</t>
-        </is>
-      </c>
+          <t>24-031264-779580762490001</t>
+        </is>
+      </c>
+      <c r="W5" t="inlineStr"/>
       <c r="X5" t="inlineStr">
         <is>
-          <t>02</t>
+          <t>(!) No se encontró coincidencia en la tabla de asignación</t>
         </is>
       </c>
       <c r="Y5" t="inlineStr">
         <is>
-          <t>16150.00</t>
+          <t>81141601</t>
         </is>
       </c>
       <c r="Z5" t="inlineStr">
         <is>
-          <t>002</t>
-        </is>
-      </c>
-      <c r="AA5" t="inlineStr">
-        <is>
-          <t>0.160000</t>
-        </is>
-      </c>
-      <c r="AB5" t="inlineStr">
-        <is>
-          <t>2584.00</t>
-        </is>
-      </c>
-      <c r="AC5" t="inlineStr">
-        <is>
-          <t>16150.00|</t>
-        </is>
-      </c>
-      <c r="AD5" t="inlineStr">
-        <is>
-          <t>002|</t>
-        </is>
-      </c>
-      <c r="AE5" t="inlineStr">
-        <is>
-          <t>0.04|</t>
-        </is>
-      </c>
-      <c r="AF5" t="inlineStr">
-        <is>
-          <t>646.00|</t>
-        </is>
-      </c>
-      <c r="AG5" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="AH5" t="inlineStr">
-        <is>
-          <t>Sin carta porte</t>
-        </is>
-      </c>
-      <c r="AI5" t="inlineStr">
-        <is>
-          <t>7f743e76-7eb5-4cb8-a576-2773178b0e8e</t>
-        </is>
-      </c>
-      <c r="AJ5" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Retención incorrecta para clave de prod. y serv.| Carta Porte no anexa para clave de prod. y serv.| </t>
+          <t>SERVICIOS DE LOGISTICA (MX)/LOGISTIC SERVICES (MX)</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix retention key assignment logic and remove redundant filters in conceptos_df function
</commit_message>
<xml_diff>
--- a/checar.xlsx
+++ b/checar.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Z5"/>
+  <dimension ref="A1:Z4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -590,7 +590,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>T00943</t>
+          <t>T00003</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -600,35 +600,35 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>24-030477</t>
+          <t>24-031491</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>MXN</t>
+          <t>USD</t>
         </is>
       </c>
       <c r="J2" t="inlineStr"/>
       <c r="K2" t="inlineStr">
         <is>
-          <t>EFDFED4B-8E21-1B43-B155-15BB076CDE38</t>
+          <t>8FCF09CC-58F1-4E6B-ADCA-CA13CD9623CA</t>
         </is>
       </c>
       <c r="L2" t="inlineStr"/>
       <c r="M2" t="inlineStr">
         <is>
-          <t>05/11/2024</t>
+          <t>01/11/2024</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>05/11/2024</t>
+          <t>01/11/2024</t>
         </is>
       </c>
       <c r="O2" t="inlineStr"/>
       <c r="P2" t="inlineStr">
         <is>
-          <t>INDETERMINADO</t>
+          <t>FLETE_TER_N</t>
         </is>
       </c>
       <c r="Q2" t="n">
@@ -636,7 +636,7 @@
       </c>
       <c r="R2" t="inlineStr">
         <is>
-          <t>1693.01</t>
+          <t>75.00</t>
         </is>
       </c>
       <c r="S2" t="inlineStr">
@@ -646,33 +646,33 @@
       </c>
       <c r="T2" t="inlineStr">
         <is>
-          <t>G1I</t>
+          <t>A3V</t>
         </is>
       </c>
       <c r="U2" t="inlineStr">
         <is>
-          <t>270.88</t>
+          <t>12.00</t>
         </is>
       </c>
       <c r="V2" t="inlineStr">
         <is>
-          <t>24-030477-779471674450001</t>
+          <t>24-031491-290519</t>
         </is>
       </c>
       <c r="W2" t="inlineStr"/>
       <c r="X2" t="inlineStr">
         <is>
-          <t>(!) No se encontró coincidencia en la tabla de asignación</t>
+          <t>Traslado y retención de IVA/ cve SAT: T. local (o con clave general) /Sin CCP</t>
         </is>
       </c>
       <c r="Y2" t="inlineStr">
         <is>
-          <t>81141601</t>
+          <t>78101801</t>
         </is>
       </c>
       <c r="Z2" t="inlineStr">
         <is>
-          <t>SERVICIOS DE LOGISTICA (MX)/LOGISTIC SERVICES (MX)</t>
+          <t>SERVICIO DE TRANSPORTE DE CARGA LOCAL REF.:24-031491</t>
         </is>
       </c>
     </row>
@@ -700,7 +700,7 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>T00943</t>
+          <t>T00003</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
@@ -710,35 +710,35 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>24-030480</t>
+          <t>24-031489</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>MXN</t>
+          <t>USD</t>
         </is>
       </c>
       <c r="J3" t="inlineStr"/>
       <c r="K3" t="inlineStr">
         <is>
-          <t>E80D77EB-575A-B645-A714-21A9A53E5255</t>
+          <t>2E7DB79F-F9F8-42CF-8039-BFC802CF1130</t>
         </is>
       </c>
       <c r="L3" t="inlineStr"/>
       <c r="M3" t="inlineStr">
         <is>
-          <t>05/11/2024</t>
+          <t>01/11/2024</t>
         </is>
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>05/11/2024</t>
+          <t>01/11/2024</t>
         </is>
       </c>
       <c r="O3" t="inlineStr"/>
       <c r="P3" t="inlineStr">
         <is>
-          <t>INDETERMINADO</t>
+          <t>FLETE_TER_N</t>
         </is>
       </c>
       <c r="Q3" t="n">
@@ -746,7 +746,7 @@
       </c>
       <c r="R3" t="inlineStr">
         <is>
-          <t>1148.99</t>
+          <t>75.00</t>
         </is>
       </c>
       <c r="S3" t="inlineStr">
@@ -756,33 +756,33 @@
       </c>
       <c r="T3" t="inlineStr">
         <is>
-          <t>G1I</t>
+          <t>A3V</t>
         </is>
       </c>
       <c r="U3" t="inlineStr">
         <is>
-          <t>183.84</t>
+          <t>12.00</t>
         </is>
       </c>
       <c r="V3" t="inlineStr">
         <is>
-          <t>24-030480-779474725969001</t>
+          <t>24-031489-290520</t>
         </is>
       </c>
       <c r="W3" t="inlineStr"/>
       <c r="X3" t="inlineStr">
         <is>
-          <t>(!) No se encontró coincidencia en la tabla de asignación</t>
+          <t>Traslado y retención de IVA/ cve SAT: T. local (o con clave general) /Sin CCP</t>
         </is>
       </c>
       <c r="Y3" t="inlineStr">
         <is>
-          <t>81141601</t>
+          <t>78101801</t>
         </is>
       </c>
       <c r="Z3" t="inlineStr">
         <is>
-          <t>SERVICIOS DE LOGISTICA (MX)/LOGISTIC SERVICES (MX)</t>
+          <t>SERVICIO DE TRANSPORTE DE CARGA LOCAL REF.:24-031489</t>
         </is>
       </c>
     </row>
@@ -810,7 +810,7 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>T00943</t>
+          <t>T00003</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
@@ -820,35 +820,35 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>24-031142</t>
+          <t>24-031490</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>MXN</t>
+          <t>USD</t>
         </is>
       </c>
       <c r="J4" t="inlineStr"/>
       <c r="K4" t="inlineStr">
         <is>
-          <t>BD665673-1EAF-4D46-A3F2-EECA0C64AC6D</t>
+          <t>CC8C6842-7097-4C01-A2FB-D34397AB06F5</t>
         </is>
       </c>
       <c r="L4" t="inlineStr"/>
       <c r="M4" t="inlineStr">
         <is>
-          <t>05/11/2024</t>
+          <t>01/11/2024</t>
         </is>
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>05/11/2024</t>
+          <t>01/11/2024</t>
         </is>
       </c>
       <c r="O4" t="inlineStr"/>
       <c r="P4" t="inlineStr">
         <is>
-          <t>INDETERMINADO</t>
+          <t>FLETE_TER_N</t>
         </is>
       </c>
       <c r="Q4" t="n">
@@ -856,7 +856,7 @@
       </c>
       <c r="R4" t="inlineStr">
         <is>
-          <t>21272.92</t>
+          <t>75.00</t>
         </is>
       </c>
       <c r="S4" t="inlineStr">
@@ -866,143 +866,33 @@
       </c>
       <c r="T4" t="inlineStr">
         <is>
-          <t>G1I</t>
+          <t>A3V</t>
         </is>
       </c>
       <c r="U4" t="inlineStr">
         <is>
-          <t>3403.67</t>
+          <t>12.00</t>
         </is>
       </c>
       <c r="V4" t="inlineStr">
         <is>
-          <t>24-031142-779567411325001</t>
+          <t>24-031490-290518</t>
         </is>
       </c>
       <c r="W4" t="inlineStr"/>
       <c r="X4" t="inlineStr">
         <is>
-          <t>(!) No se encontró coincidencia en la tabla de asignación</t>
+          <t>Traslado y retención de IVA/ cve SAT: T. local (o con clave general) /Sin CCP</t>
         </is>
       </c>
       <c r="Y4" t="inlineStr">
         <is>
-          <t>81141601</t>
+          <t>78101801</t>
         </is>
       </c>
       <c r="Z4" t="inlineStr">
         <is>
-          <t>SERVICIOS DE LOGISTICA (MX)/LOGISTIC SERVICES (MX)</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>4</v>
-      </c>
-      <c r="B5" t="n">
-        <v>1</v>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Factura</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>CC</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>MLG1405</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>T00943</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>MLG1000</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>24-031264</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>MXN</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr"/>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>AA872B02-4680-B54D-A486-0E8C3905A4B3</t>
-        </is>
-      </c>
-      <c r="L5" t="inlineStr"/>
-      <c r="M5" t="inlineStr">
-        <is>
-          <t>05/11/2024</t>
-        </is>
-      </c>
-      <c r="N5" t="inlineStr">
-        <is>
-          <t>05/11/2024</t>
-        </is>
-      </c>
-      <c r="O5" t="inlineStr"/>
-      <c r="P5" t="inlineStr">
-        <is>
-          <t>INDETERMINADO</t>
-        </is>
-      </c>
-      <c r="Q5" t="n">
-        <v>1</v>
-      </c>
-      <c r="R5" t="inlineStr">
-        <is>
-          <t>1593.50</t>
-        </is>
-      </c>
-      <c r="S5" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="T5" t="inlineStr">
-        <is>
-          <t>G1I</t>
-        </is>
-      </c>
-      <c r="U5" t="inlineStr">
-        <is>
-          <t>254.96</t>
-        </is>
-      </c>
-      <c r="V5" t="inlineStr">
-        <is>
-          <t>24-031264-779580762490001</t>
-        </is>
-      </c>
-      <c r="W5" t="inlineStr"/>
-      <c r="X5" t="inlineStr">
-        <is>
-          <t>(!) No se encontró coincidencia en la tabla de asignación</t>
-        </is>
-      </c>
-      <c r="Y5" t="inlineStr">
-        <is>
-          <t>81141601</t>
-        </is>
-      </c>
-      <c r="Z5" t="inlineStr">
-        <is>
-          <t>SERVICIOS DE LOGISTICA (MX)/LOGISTIC SERVICES (MX)</t>
+          <t>SERVICIO DE TRANSPORTE DE CARGA LOCAL REF.:24-031490</t>
         </is>
       </c>
     </row>

</xml_diff>